<commit_message>
fix bug for sub_list and item_number
</commit_message>
<xml_diff>
--- a/new_graph_build/updated.xlsx
+++ b/new_graph_build/updated.xlsx
@@ -589,7 +589,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>局部治疗,病灶,中枢神经系统转移</t>
+          <t>病灶,中枢神经系统转移,局部治疗</t>
         </is>
       </c>
       <c r="K3" t="inlineStr"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>活检,切片</t>
+          <t>切片,活检</t>
         </is>
       </c>
       <c r="K4" t="inlineStr"/>
@@ -748,7 +748,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>胸腔积液,腹水,心包积液,前三个月,洗脱期</t>
+          <t>胸腔积液,心包积液,洗脱期,前三个月,腹水</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -852,7 +852,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>突变,一线治疗,KRAS</t>
+          <t>一线治疗,KRAS,突变</t>
         </is>
       </c>
       <c r="K8" t="inlineStr"/>
@@ -907,7 +907,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>辅助治疗,6个月,洗脱期</t>
+          <t>辅助治疗,洗脱期,6个月</t>
         </is>
       </c>
       <c r="K9" t="inlineStr"/>
@@ -981,7 +981,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>感染,ILD,类固醇,炎症</t>
+          <t>炎症,感染,类固醇,ILD</t>
         </is>
       </c>
       <c r="K11" t="inlineStr"/>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>第4,局部治疗,方案,中枢神经系统转移,T-DXd,脑转移</t>
+          <t>T-DXd,第4,方案,局部治疗,脑转移,中枢神经系统转移</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>毒性,禁忌症,帕博利珠,铂,免疫,MP相关,自身免疫,医学禁忌</t>
+          <t>MP相关,铂,毒性,免疫,禁忌症,帕博利珠,自身免疫,医学禁忌</t>
         </is>
       </c>
       <c r="K13" t="inlineStr"/>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>一线治疗,突变,HER2突变,人群</t>
+          <t>人群,HER2突变,一线治疗,突变</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>肿瘤样本,突变,样本,方案</t>
+          <t>方案,样本,肿瘤样本,突变</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>数据且,突变,EGFR,方案,ROS1、PDL1,ctDNA,ALK</t>
+          <t>ctDNA,EGFR,突变,数据且,方案,ROS1、PDL1,ALK</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>靶病灶,局部治疗,病灶,中枢神经系统转移,RECIST</t>
+          <t>靶病灶,病灶,局部治疗,中枢神经系统转移,RECIST</t>
         </is>
       </c>
       <c r="K17" t="inlineStr"/>
@@ -1352,7 +1352,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>胸腔积液,肺炎,腹水,T-DXd,心包积液,肺癌,洗脱期</t>
+          <t>胸腔积液,心包积液,洗脱期,T-DXd,肺炎,肺癌,腹水</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>突变,方案,基因突变,基因,HER2突变,基因组,ctDNA,HER2</t>
+          <t>HER2,基因组,ctDNA,突变,基因突变,方案,基因,HER2突变</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>治疗洗脱期,洗脱期,方案</t>
+          <t>方案,洗脱期,治疗洗脱期</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>治疗洗脱期,洗脱期,方案</t>
+          <t>方案,洗脱期,治疗洗脱期</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2周,洗脱期</t>
+          <t>洗脱期,2周</t>
         </is>
       </c>
       <c r="K24" t="inlineStr"/>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>穿刺,胸腔积液,洗脱期</t>
+          <t>胸腔积液,洗脱期,穿刺</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>穿刺,胸腔积液,洗脱期</t>
+          <t>胸腔积液,洗脱期,穿刺</t>
         </is>
       </c>
       <c r="K26" t="inlineStr"/>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>穿刺,胸腔积液,洗脱期</t>
+          <t>胸腔积液,洗脱期,穿刺</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>局部治疗,方案,日本,中枢神经系统转移,CNS,CNS转移</t>
+          <t>日本,CNS转移,方案,局部治疗,CNS,中枢神经系统转移</t>
         </is>
       </c>
       <c r="K28" t="inlineStr"/>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>ICF,临床研究,第21,临床试验,观察性</t>
+          <t>观察性,ICF,临床试验,临床研究,第21</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
@@ -2203,7 +2203,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>组织学类型,腺癌,小细胞肺癌</t>
+          <t>腺癌,组织学类型,小细胞肺癌</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2个月,切片,肿瘤组织,6个月,样本</t>
+          <t>2个月,肿瘤组织,切片,样本,6个月</t>
         </is>
       </c>
       <c r="K39" t="inlineStr"/>
@@ -2723,7 +2723,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>方案,胸腔积液,ICF,两周,洗脱期</t>
+          <t>胸腔积液,ICF,洗脱期,方案,两周</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
@@ -2824,7 +2824,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>突变,莫博替尼,EGFR,日本,美国,ALK</t>
+          <t>EGFR,突变,美国,莫博替尼,日本,ALK</t>
         </is>
       </c>
       <c r="K49" t="inlineStr"/>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>T-DXd,ICF</t>
+          <t>ICF,T-DXd</t>
         </is>
       </c>
       <c r="K50" t="inlineStr"/>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>IV期,放疗,根治性治疗</t>
+          <t>根治性治疗,放疗,IV期</t>
         </is>
       </c>
       <c r="K51" t="inlineStr"/>
@@ -2980,7 +2980,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>IV期,放疗,根治性治疗</t>
+          <t>根治性治疗,放疗,IV期</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>组织学类型,腺癌,小细胞肺癌</t>
+          <t>腺癌,组织学类型,小细胞肺癌</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
@@ -3083,7 +3083,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>MSUD,T-DXd,代谢失,感染</t>
+          <t>代谢失,MSUD,感染,T-DXd</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
@@ -3308,7 +3308,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>中枢神经系统,脑转移,洗脱期,ICF</t>
+          <t>ICF,洗脱期,脑转移,中枢神经系统</t>
         </is>
       </c>
       <c r="K59" t="inlineStr"/>
@@ -3360,7 +3360,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>一线治疗,姑息性全身治疗,6个月后,方案,3周,局部晚期,6个月,铂,免疫,全身治疗,洗脱期,铂类</t>
+          <t>一线治疗,洗脱期,姑息性全身治疗,铂,全身治疗,3周,方案,局部晚期,铂类,免疫,6个月,6个月后</t>
         </is>
       </c>
       <c r="K60" t="inlineStr"/>
@@ -3406,7 +3406,7 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
-          <t>一周,前一周,方案</t>
+          <t>一周,方案,前一周</t>
         </is>
       </c>
       <c r="K61" t="inlineStr"/>

</xml_diff>